<commit_message>
continue population sims and plots
</commit_message>
<xml_diff>
--- a/BMUS_LH_sim_pop_parameters.xlsx
+++ b/BMUS_LH_sim_pop_parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erin.Bohaboy\Documents\CNMI\NMarianas_Cruise_Jul2025\CNMI_unfished_sampling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20B496A9-6521-48CE-82CD-8774612C0D45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E09B307-8A76-43B4-9EC1-2C995E4829AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-72" windowWidth="23256" windowHeight="12576" xr2:uid="{9042A815-CDAD-4DE4-BECF-BDB7D52D9E40}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{9042A815-CDAD-4DE4-BECF-BDB7D52D9E40}"/>
   </bookViews>
   <sheets>
     <sheet name="parms" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Parameter</t>
   </si>
@@ -46,9 +46,6 @@
     <t>APRU</t>
   </si>
   <si>
-    <t>CALU</t>
-  </si>
-  <si>
     <t>ETCA</t>
   </si>
   <si>
@@ -62,9 +59,6 @@
   </si>
   <si>
     <t>PRZO</t>
-  </si>
-  <si>
-    <t>VALO</t>
   </si>
   <si>
     <t>Linf</t>
@@ -467,10 +461,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8956B189-10CE-47B9-97C5-4ED1527C9038}">
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -479,7 +473,7 @@
     <col min="2" max="2" width="10.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -490,10 +484,10 @@
         <v>3</v>
       </c>
       <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
         <v>4</v>
-      </c>
-      <c r="E1" t="s">
-        <v>1</v>
       </c>
       <c r="F1" t="s">
         <v>5</v>
@@ -504,146 +498,446 @@
       <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="B2">
+        <v>92.9</v>
+      </c>
+      <c r="C2">
+        <v>49</v>
+      </c>
+      <c r="D2">
+        <v>100</v>
+      </c>
+      <c r="E2">
+        <v>35.9</v>
+      </c>
+      <c r="F2">
+        <v>54.5</v>
+      </c>
+      <c r="G2">
+        <v>42.9</v>
+      </c>
+      <c r="H2">
+        <v>37.700000000000003</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="B3">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="C3">
+        <v>1.2</v>
+      </c>
+      <c r="D3">
+        <v>2.5</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>1.4</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>10</v>
       </c>
-      <c r="E2">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="B4">
+        <v>0.19400000000000001</v>
+      </c>
+      <c r="C4">
+        <v>0.2</v>
+      </c>
+      <c r="D4">
+        <v>0.125</v>
+      </c>
+      <c r="E4">
+        <v>0.20499999999999999</v>
+      </c>
+      <c r="F4">
+        <v>0.13600000000000001</v>
+      </c>
+      <c r="G4">
+        <v>0.23100000000000001</v>
+      </c>
+      <c r="H4">
+        <v>0.17499999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>11</v>
       </c>
-      <c r="E3">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>12</v>
       </c>
-      <c r="E4">
-        <v>0.125</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="B6" t="b">
+        <v>1</v>
+      </c>
+      <c r="C6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D6" t="b">
+        <v>1</v>
+      </c>
+      <c r="E6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F6" t="b">
+        <v>1</v>
+      </c>
+      <c r="G6" t="b">
+        <v>1</v>
+      </c>
+      <c r="H6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>13</v>
       </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>15</v>
+      <c r="B7">
+        <v>10</v>
+      </c>
+      <c r="C7">
+        <v>10</v>
+      </c>
+      <c r="D7">
+        <v>10</v>
       </c>
       <c r="E7">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="F7">
+        <v>10</v>
+      </c>
+      <c r="G7">
+        <v>10</v>
+      </c>
+      <c r="H7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>14</v>
+      </c>
+      <c r="B8">
+        <v>2.5</v>
+      </c>
+      <c r="C8">
+        <v>2.5</v>
+      </c>
+      <c r="D8">
+        <v>2.5</v>
       </c>
       <c r="E8">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="F8">
+        <v>2.5</v>
+      </c>
+      <c r="G8">
+        <v>2.5</v>
+      </c>
+      <c r="H8">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>15</v>
+      </c>
+      <c r="B9">
+        <v>200</v>
+      </c>
+      <c r="C9">
+        <v>200</v>
+      </c>
+      <c r="D9">
+        <v>200</v>
       </c>
       <c r="E9">
         <v>200</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="F9">
+        <v>200</v>
+      </c>
+      <c r="G9">
+        <v>200</v>
+      </c>
+      <c r="H9">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11">
+        <v>2</v>
+      </c>
+      <c r="C11">
+        <v>9.66</v>
+      </c>
+      <c r="D11">
+        <v>10</v>
+      </c>
+      <c r="E11">
+        <v>15</v>
+      </c>
+      <c r="F11">
+        <v>17.5</v>
+      </c>
+      <c r="G11">
+        <v>13.3</v>
+      </c>
+      <c r="H11">
+        <v>13.6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
         <v>18</v>
       </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+      <c r="B12">
+        <v>0.5</v>
+      </c>
+      <c r="C12">
+        <v>2.42</v>
+      </c>
+      <c r="D12">
+        <v>2.5</v>
+      </c>
+      <c r="E12">
+        <v>3.75</v>
+      </c>
+      <c r="F12">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="G12">
+        <v>3.3</v>
+      </c>
+      <c r="H12">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
         <v>19</v>
       </c>
-      <c r="E11">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
+      <c r="B13">
+        <v>0.17</v>
+      </c>
+      <c r="C13">
+        <v>0.22</v>
+      </c>
+      <c r="D13">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="E13">
+        <v>0.54</v>
+      </c>
+      <c r="F13">
+        <v>0.2</v>
+      </c>
+      <c r="G13">
+        <v>0.37</v>
+      </c>
+      <c r="H13">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
         <v>20</v>
       </c>
-      <c r="E12">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
+      <c r="B14">
+        <v>0.01</v>
+      </c>
+      <c r="C14">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="D14">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="E14">
+        <v>3.1E-2</v>
+      </c>
+      <c r="F14">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="G14">
+        <v>0.02</v>
+      </c>
+      <c r="H14">
+        <v>1.4E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
         <v>21</v>
       </c>
-      <c r="E13">
-        <v>0.14000000000000001</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
+      <c r="B15">
+        <v>34</v>
+      </c>
+      <c r="C15">
+        <v>33</v>
+      </c>
+      <c r="D15">
+        <v>55</v>
+      </c>
+      <c r="E15">
+        <v>32</v>
+      </c>
+      <c r="F15">
+        <v>50</v>
+      </c>
+      <c r="G15">
+        <v>28</v>
+      </c>
+      <c r="H15">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
         <v>22</v>
       </c>
-      <c r="E14">
-        <v>8.0000000000000002E-3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>23</v>
-      </c>
-      <c r="E15">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>24</v>
+      <c r="B16">
+        <v>20</v>
+      </c>
+      <c r="C16">
+        <v>20</v>
+      </c>
+      <c r="D16">
+        <v>20</v>
       </c>
       <c r="E16">
         <v>20</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F16">
+        <v>20</v>
+      </c>
+      <c r="G16">
+        <v>20</v>
+      </c>
+      <c r="H16">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>25</v>
+        <v>23</v>
+      </c>
+      <c r="B17">
+        <v>100000</v>
+      </c>
+      <c r="C17">
+        <v>100000</v>
+      </c>
+      <c r="D17">
+        <v>50000</v>
       </c>
       <c r="E17">
         <v>100000</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F17">
+        <v>100000</v>
+      </c>
+      <c r="G17">
+        <v>100000</v>
+      </c>
+      <c r="H17">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>26</v>
+        <v>24</v>
+      </c>
+      <c r="B18" t="b">
+        <v>1</v>
+      </c>
+      <c r="C18" t="b">
+        <v>1</v>
+      </c>
+      <c r="D18" t="b">
+        <v>1</v>
       </c>
       <c r="E18" t="b">
+        <v>1</v>
+      </c>
+      <c r="F18" t="b">
+        <v>1</v>
+      </c>
+      <c r="G18" t="b">
+        <v>1</v>
+      </c>
+      <c r="H18" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
simulating pops and adding plotting
</commit_message>
<xml_diff>
--- a/BMUS_LH_sim_pop_parameters.xlsx
+++ b/BMUS_LH_sim_pop_parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erin.Bohaboy\Documents\CNMI\NMarianas_Cruise_Jul2025\CNMI_unfished_sampling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E09B307-8A76-43B4-9EC1-2C995E4829AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4E44B7A-E3FF-45E1-A141-A1C0CF691A38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{9042A815-CDAD-4DE4-BECF-BDB7D52D9E40}"/>
   </bookViews>
@@ -464,7 +464,7 @@
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -894,25 +894,25 @@
         <v>23</v>
       </c>
       <c r="B17">
-        <v>100000</v>
+        <v>500000</v>
       </c>
       <c r="C17">
-        <v>100000</v>
+        <v>500000</v>
       </c>
       <c r="D17">
-        <v>50000</v>
+        <v>500000</v>
       </c>
       <c r="E17">
-        <v>100000</v>
+        <v>500000</v>
       </c>
       <c r="F17">
-        <v>100000</v>
+        <v>500000</v>
       </c>
       <c r="G17">
-        <v>100000</v>
+        <v>500000</v>
       </c>
       <c r="H17">
-        <v>100000</v>
+        <v>500000</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
add R markdown to show simulated populations
</commit_message>
<xml_diff>
--- a/BMUS_LH_sim_pop_parameters.xlsx
+++ b/BMUS_LH_sim_pop_parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erin.Bohaboy\Documents\CNMI\NMarianas_Cruise_Jul2025\CNMI_unfished_sampling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4E44B7A-E3FF-45E1-A141-A1C0CF691A38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0821C543-C908-466D-94BF-46DF5952E253}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{9042A815-CDAD-4DE4-BECF-BDB7D52D9E40}"/>
   </bookViews>
@@ -464,7 +464,7 @@
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -894,25 +894,25 @@
         <v>23</v>
       </c>
       <c r="B17">
-        <v>500000</v>
+        <v>100000</v>
       </c>
       <c r="C17">
-        <v>500000</v>
+        <v>100000</v>
       </c>
       <c r="D17">
-        <v>500000</v>
+        <v>100000</v>
       </c>
       <c r="E17">
-        <v>500000</v>
+        <v>100000</v>
       </c>
       <c r="F17">
-        <v>500000</v>
+        <v>100000</v>
       </c>
       <c r="G17">
-        <v>500000</v>
+        <v>100000</v>
       </c>
       <c r="H17">
-        <v>500000</v>
+        <v>100000</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">

</xml_diff>